<commit_message>
Updated Bertin roughing notebook
</commit_message>
<xml_diff>
--- a/substrates_template.xlsx
+++ b/substrates_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fauchere\Documents\02-Programmes\Python\scripts\solar_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9B009F-6C5C-41E1-9254-4131A43A28AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B62413-6364-4DBA-BC6B-4843798D74EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1290,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1338,7 +1338,7 @@
         <v>22</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Added support for mirror crown angles
</commit_message>
<xml_diff>
--- a/substrates_template.xlsx
+++ b/substrates_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fauchere\Documents\02-Programmes\Python\scripts\solar_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B62413-6364-4DBA-BC6B-4843798D74EF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084E6A9-4FA2-4B96-B534-27BDEFB34D98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
   <si>
     <t>File</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>LW_rectangle_20250425_003.asc</t>
+  </si>
+  <si>
+    <t>crown index</t>
   </si>
 </sst>
 </file>
@@ -917,6 +920,13 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -926,13 +936,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1290,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1302,13 +1305,14 @@
     <col min="4" max="4" width="11.86328125" style="1" customWidth="1"/>
     <col min="5" max="5" width="12.265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="12" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.06640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9" style="1"/>
+    <col min="7" max="7" width="8.73046875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1348,21 +1352,21 @@
       </c>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="30" t="s">
+    <row r="4" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="26" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="26"/>
+      <c r="B6" s="31"/>
     </row>
     <row r="7" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="8" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="27" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1400,9 +1404,9 @@
         <v>-13.225</v>
       </c>
     </row>
-    <row r="11" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="31" t="s">
+    <row r="11" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="28" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1440,9 +1444,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="1:6" s="31" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="31" t="s">
+    <row r="15" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="28" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1494,7 +1498,7 @@
       <c r="L18" s="20"/>
       <c r="M18" s="20"/>
     </row>
-    <row r="19" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="19" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="23" t="s">
         <v>69</v>
@@ -1541,8 +1545,8 @@
       </c>
     </row>
     <row r="23" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="26" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1574,107 +1578,116 @@
         <v>-13.225</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:13" s="30" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="30" t="s">
+    <row r="27" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="26" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="33" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="29" t="s">
+    <row r="31" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="27" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="8" t="s">
+    <row r="33" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="C33" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="E33" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="G33" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="H33" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H33" s="8" t="s">
+      <c r="I33" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A34" s="6">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A34" s="5">
+        <v>5</v>
+      </c>
+      <c r="B34" s="6">
         <v>154.56</v>
       </c>
-      <c r="B34" s="6">
+      <c r="C34" s="6">
         <v>911.77</v>
       </c>
-      <c r="C34" s="6">
+      <c r="D34" s="6">
         <v>621.72</v>
       </c>
-      <c r="D34" s="6">
+      <c r="E34" s="6">
         <v>256.61</v>
       </c>
-      <c r="E34" s="6">
+      <c r="F34" s="6">
         <v>1077.94</v>
       </c>
-      <c r="F34" s="6">
+      <c r="G34" s="6">
         <v>911.91</v>
       </c>
-      <c r="G34" s="6">
+      <c r="H34" s="6">
         <v>4</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="I34" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5">
         <v>292.89</v>
       </c>
-      <c r="B35" s="5">
+      <c r="C35" s="5">
         <v>1043.42</v>
       </c>
-      <c r="C35" s="5">
+      <c r="D35" s="5">
         <v>946.29</v>
       </c>
-      <c r="D35" s="5">
+      <c r="E35" s="5">
         <v>587.9</v>
       </c>
-      <c r="E35" s="5">
+      <c r="F35" s="5">
         <v>295.33</v>
       </c>
-      <c r="F35" s="5">
+      <c r="G35" s="5">
         <v>126.69</v>
       </c>
-      <c r="G35" s="6">
+      <c r="H35" s="6">
         <v>4</v>
       </c>
-      <c r="H35" s="5" t="s">
+      <c r="I35" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1683,8 +1696,9 @@
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1693,8 +1707,9 @@
       <c r="F37" s="5"/>
       <c r="G37" s="6"/>
       <c r="H37" s="5"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1703,8 +1718,9 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1713,8 +1729,9 @@
       <c r="F39" s="5"/>
       <c r="G39" s="6"/>
       <c r="H39" s="5"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1723,8 +1740,9 @@
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1733,8 +1751,9 @@
       <c r="F41" s="5"/>
       <c r="G41" s="6"/>
       <c r="H41" s="5"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1743,8 +1762,9 @@
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1753,8 +1773,9 @@
       <c r="F43" s="5"/>
       <c r="G43" s="6"/>
       <c r="H43" s="5"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1763,8 +1784,9 @@
       <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1773,6 +1795,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="6"/>
       <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.45">
       <c r="C154" s="7"/>
@@ -1780,6 +1803,10 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="17">
+    <mergeCell ref="A31:XFD31"/>
+    <mergeCell ref="A30:XFD30"/>
+    <mergeCell ref="A29:XFD29"/>
+    <mergeCell ref="A32:XFD32"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A24:XFD24"/>
     <mergeCell ref="A28:XFD28"/>
@@ -1793,16 +1820,12 @@
     <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A5:XFD5"/>
     <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A31:XFD31"/>
-    <mergeCell ref="A30:XFD30"/>
-    <mergeCell ref="A29:XFD29"/>
-    <mergeCell ref="A32:XFD32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD697CB8-BC54-434F-A65F-3DDD7DCD54FC}">
           <x14:formula1>
             <xm:f>options!$B$2:$B$3</xm:f>

</xml_diff>

<commit_message>
Comments in susbstrate template
</commit_message>
<xml_diff>
--- a/substrates_template.xlsx
+++ b/substrates_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fauchere\Documents\02-Programmes\Python\scripts\solar_c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B084E6A9-4FA2-4B96-B534-27BDEFB34D98}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2968AABB-083E-4D08-8FC6-FEFCBC07DBBD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7680" windowHeight="3413" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fit" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
   <si>
     <t>File</t>
   </si>
@@ -158,9 +158,6 @@
     <t>k</t>
   </si>
   <si>
-    <t>RectangularAperture</t>
-  </si>
-  <si>
     <t>Aperture</t>
   </si>
   <si>
@@ -168,9 +165,6 @@
   </si>
   <si>
     <t>UsefulArea</t>
-  </si>
-  <si>
-    <t>PieAperture</t>
   </si>
   <si>
     <t>dz [mm]</t>
@@ -270,9 +264,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>k [mm]</t>
   </si>
   <si>
@@ -325,6 +316,32 @@
   </si>
   <si>
     <t>crown index</t>
+  </si>
+  <si>
+    <t>Useful area over which th fit is performed</t>
+  </si>
+  <si>
+    <t>Measured position of the three fiducials in the EGA reference frame</t>
+  </si>
+  <si>
+    <t>Initial reference wavefront used for the fit.</t>
+  </si>
+  <si>
+    <t>(x1, y1), (x2, y2), (x3, y3) are the coordinates in pixels of the three fiducials. Their order with respect to the definition in 2.4 does not matter.
+Binning defines the rebinnined performed on the data prior to fitting, not how much the data was binned during the acquisition.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surface fitting options
+</t>
+  </si>
+  <si>
+    <t>Nominal shape of the susbstrate (in Zemax notations)</t>
+  </si>
+  <si>
+    <t>Outer dimensions of the substrate. Must include the useful area but  the exact shape is not critical.</t>
+  </si>
+  <si>
+    <t>radius [mm]</t>
   </si>
 </sst>
 </file>
@@ -668,7 +685,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -811,6 +828,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -856,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -904,9 +930,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -920,6 +943,8 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
@@ -927,14 +952,37 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1291,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M154"/>
+  <dimension ref="A1:O154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1311,12 +1359,12 @@
     <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
@@ -1332,9 +1380,17 @@
       <c r="E2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F2" s="21"/>
+      <c r="J2" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>1.0000000000000001E-9</v>
       </c>
@@ -1351,26 +1407,38 @@
         <v>6</v>
       </c>
       <c r="F3" s="20"/>
-    </row>
-    <row r="4" spans="1:6" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="5" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="26" t="s">
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+    </row>
+    <row r="4" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="5" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="31"/>
-    </row>
-    <row r="7" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="8" spans="1:6" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="27" t="s">
+    <row r="6" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" s="25"/>
+      <c r="J6" s="26"/>
+      <c r="K6" s="26"/>
+      <c r="L6" s="26"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+    </row>
+    <row r="7" spans="1:15" s="41" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="8" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1446,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D9" s="8" t="s">
         <v>33</v>
@@ -1386,8 +1454,16 @@
       <c r="E9" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J9" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+    </row>
+    <row r="10" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="13" t="s">
         <v>2</v>
       </c>
@@ -1403,14 +1479,20 @@
       <c r="E10" s="12">
         <v>-13.225</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="12" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="28" t="s">
+      <c r="J10" s="34"/>
+      <c r="K10" s="34"/>
+      <c r="L10" s="34"/>
+      <c r="M10" s="34"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
+    </row>
+    <row r="11" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="12" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="29" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>7</v>
       </c>
@@ -1426,8 +1508,16 @@
       <c r="E13" s="9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J13" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
+    </row>
+    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A14" s="13" t="s">
         <v>36</v>
       </c>
@@ -1443,14 +1533,20 @@
       <c r="E14" s="12">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="16" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="28" t="s">
+      <c r="J14" s="34"/>
+      <c r="K14" s="34"/>
+      <c r="L14" s="34"/>
+      <c r="M14" s="34"/>
+      <c r="N14" s="34"/>
+      <c r="O14" s="34"/>
+    </row>
+    <row r="15" spans="1:15" s="31" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="16" spans="1:15" s="29" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="29" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>7</v>
       </c>
@@ -1469,12 +1565,16 @@
       <c r="F17" s="19"/>
       <c r="H17" s="19"/>
       <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J17" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36"/>
+      <c r="N17" s="36"/>
+      <c r="O17" s="36"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" s="13" t="s">
         <v>36</v>
       </c>
@@ -1493,38 +1593,48 @@
       <c r="F18" s="20"/>
       <c r="H18" s="20"/>
       <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="20"/>
-      <c r="M18" s="20"/>
-    </row>
-    <row r="19" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="20" spans="1:13" s="23" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="23" t="s">
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+    </row>
+    <row r="19" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="20" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A21" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="25" t="s">
+      <c r="D21" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="E21" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="F21" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>74</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" s="24" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="J21" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="39"/>
+      <c r="L21" s="39"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="39"/>
+      <c r="O21" s="39"/>
+    </row>
+    <row r="22" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>-17.925000000000001</v>
       </c>
@@ -1543,14 +1653,20 @@
       <c r="F22" s="6">
         <v>-41.094000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="26" t="s">
+      <c r="J22" s="39"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="39"/>
+      <c r="O22" s="39"/>
+    </row>
+    <row r="23" spans="1:15" s="40" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="24" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A24" s="27" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="8" t="s">
         <v>9</v>
       </c>
@@ -1563,8 +1679,16 @@
       <c r="D25" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="J25" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
+      <c r="O25" s="34"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>3</v>
       </c>
@@ -1577,50 +1701,56 @@
       <c r="D26" s="5">
         <v>-13.225</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" s="29" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="28" spans="1:13" s="26" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="26" t="s">
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="34"/>
+    </row>
+    <row r="27" spans="1:15" s="30" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="28" spans="1:15" s="27" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="27" t="s">
+    <row r="29" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A29" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="33" t="s">
+    <row r="30" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="37" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="32" spans="1:15" s="28" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A33" s="12" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" s="32" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="32" spans="1:13" s="27" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A33" s="12" t="s">
-        <v>85</v>
-      </c>
       <c r="B33" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="G33" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>81</v>
       </c>
       <c r="H33" s="9" t="s">
         <v>26</v>
@@ -1628,8 +1758,16 @@
       <c r="I33" s="8" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J33" s="32" t="s">
+        <v>86</v>
+      </c>
+      <c r="K33" s="33"/>
+      <c r="L33" s="33"/>
+      <c r="M33" s="33"/>
+      <c r="N33" s="33"/>
+      <c r="O33" s="33"/>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" s="5">
         <v>5</v>
       </c>
@@ -1655,10 +1793,16 @@
         <v>4</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+        <v>80</v>
+      </c>
+      <c r="J34" s="32"/>
+      <c r="K34" s="33"/>
+      <c r="L34" s="33"/>
+      <c r="M34" s="33"/>
+      <c r="N34" s="33"/>
+      <c r="O34" s="33"/>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" s="5">
         <v>1</v>
       </c>
@@ -1684,10 +1828,16 @@
         <v>4</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+        <v>81</v>
+      </c>
+      <c r="J35" s="32"/>
+      <c r="K35" s="33"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="33"/>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1697,8 +1847,14 @@
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
       <c r="I36" s="5"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J36" s="32"/>
+      <c r="K36" s="33"/>
+      <c r="L36" s="33"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="33"/>
+      <c r="O36" s="33"/>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1708,8 +1864,14 @@
       <c r="G37" s="6"/>
       <c r="H37" s="5"/>
       <c r="I37" s="5"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J37" s="32"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
+      <c r="O37" s="33"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
@@ -1719,8 +1881,14 @@
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
       <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="J38" s="32"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="33"/>
+      <c r="N38" s="33"/>
+      <c r="O38" s="33"/>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" s="5"/>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
@@ -1731,7 +1899,7 @@
       <c r="H39" s="5"/>
       <c r="I39" s="5"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" s="5"/>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1742,7 +1910,7 @@
       <c r="H40" s="5"/>
       <c r="I40" s="5"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" s="5"/>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
@@ -1753,7 +1921,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
@@ -1764,7 +1932,7 @@
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
@@ -1775,7 +1943,7 @@
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" s="5"/>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -1786,7 +1954,7 @@
       <c r="H44" s="5"/>
       <c r="I44" s="5"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" s="5"/>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
@@ -1802,11 +1970,18 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="17">
+  <mergeCells count="25">
+    <mergeCell ref="J33:O38"/>
+    <mergeCell ref="J9:O10"/>
+    <mergeCell ref="J13:O14"/>
+    <mergeCell ref="J17:O18"/>
     <mergeCell ref="A31:XFD31"/>
     <mergeCell ref="A30:XFD30"/>
     <mergeCell ref="A29:XFD29"/>
     <mergeCell ref="A32:XFD32"/>
+    <mergeCell ref="J21:O22"/>
+    <mergeCell ref="J25:O26"/>
+    <mergeCell ref="A23:XFD23"/>
     <mergeCell ref="A1:XFD1"/>
     <mergeCell ref="A24:XFD24"/>
     <mergeCell ref="A28:XFD28"/>
@@ -1819,13 +1994,14 @@
     <mergeCell ref="A27:XFD27"/>
     <mergeCell ref="A12:XFD12"/>
     <mergeCell ref="A5:XFD5"/>
-    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="J2:O3"/>
+    <mergeCell ref="A7:XFD7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD697CB8-BC54-434F-A65F-3DDD7DCD54FC}">
           <x14:formula1>
             <xm:f>options!$B$2:$B$3</xm:f>
@@ -1872,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2EEFA51-2F97-433D-B753-B3D8C1EFBAFD}">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1955,47 +2131,47 @@
     </row>
     <row r="6" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -2005,7 +2181,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.45">
@@ -2013,13 +2189,13 @@
         <v>9</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>33</v>
@@ -2028,16 +2204,16 @@
         <v>15</v>
       </c>
       <c r="G18" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="I18" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="J18" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -2088,7 +2264,7 @@
         <v>15</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.45">
@@ -2104,13 +2280,13 @@
       <c r="D22" s="15">
         <v>-1.1539999999999999</v>
       </c>
-      <c r="E22" s="15" t="s">
-        <v>67</v>
+      <c r="E22" s="15">
+        <v>-5.8000000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
@@ -2132,7 +2308,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" s="15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B26" s="15">
         <v>17.399999999999999</v>
@@ -2167,7 +2343,7 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" s="15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B29" s="15">
         <v>61.924999999999997</v>
@@ -2185,7 +2361,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.45">
@@ -2193,7 +2369,7 @@
         <v>9</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>38</v>
@@ -2204,11 +2380,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B33" s="15">
-        <f>34.2/2</f>
-        <v>17.100000000000001</v>
+        <v>18.5</v>
       </c>
       <c r="C33" s="15">
         <v>90</v>
@@ -2224,7 +2399,7 @@
     </row>
     <row r="36" spans="1:9" s="14" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A36" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.45">
@@ -2244,16 +2419,16 @@
         <v>15</v>
       </c>
       <c r="F37" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G37" s="15" t="s">
+      <c r="I37" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="I37" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.45">
@@ -2299,7 +2474,7 @@
         <v>15</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.45">
@@ -2321,7 +2496,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.45">
@@ -2338,12 +2513,12 @@
         <v>33</v>
       </c>
       <c r="E44" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B45" s="15">
         <v>17.399999999999999</v>
@@ -2373,12 +2548,12 @@
         <v>33</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B48" s="15">
         <v>61.924999999999997</v>
@@ -2396,7 +2571,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -2404,7 +2579,7 @@
         <v>7</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>16</v>
+        <v>90</v>
       </c>
       <c r="C51" s="16" t="s">
         <v>38</v>
@@ -2416,11 +2591,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" s="15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B52" s="15">
-        <f>34.2/2</f>
-        <v>17.100000000000001</v>
+        <v>18.5</v>
       </c>
       <c r="C52" s="16">
         <v>-90</v>

</xml_diff>